<commit_message>
Adding final code version with i2c ldr resistors and 7 seg interface
</commit_message>
<xml_diff>
--- a/record.xlsx
+++ b/record.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
   <si>
     <t>Main Components with Price for 2 prototypes</t>
   </si>
@@ -170,6 +170,18 @@
   </si>
   <si>
     <t>https://circuitdigest.com/microcontroller-projects/interfacing-16x2-lcd-with-esp32-using-i2c</t>
+  </si>
+  <si>
+    <t>7-Segment Display Interfacing with Arduino UNO</t>
+  </si>
+  <si>
+    <t>https://www.electronicwings.com/arduino/7-segment-display-interfacing-with-arduino-uno</t>
+  </si>
+  <si>
+    <t>Serially Interfaced, 8-Digit, LED Display Drivers</t>
+  </si>
+  <si>
+    <t>https://www.maximintegrated.com/en/products/power/display-power-control/MAX7221.html</t>
   </si>
 </sst>
 </file>
@@ -178,10 +190,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -239,8 +251,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,11 +280,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -277,6 +304,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -284,16 +318,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -309,37 +335,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -353,7 +349,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -368,12 +364,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -402,25 +414,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,43 +570,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,102 +589,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -973,11 +985,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -987,6 +1005,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1006,32 +1039,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1053,174 +1067,172 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="33" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1281,9 +1293,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1320,9 +1329,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1334,12 +1340,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -1914,162 +1914,162 @@
       </c>
     </row>
     <row r="6" ht="37" customHeight="1" spans="2:5">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="49" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1" spans="2:5">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="55">
+      <c r="C7" s="51">
         <v>2</v>
       </c>
-      <c r="D7" s="55">
+      <c r="D7" s="51">
         <v>200</v>
       </c>
-      <c r="E7" s="56">
+      <c r="E7" s="52">
         <v>400</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1" spans="1:5">
-      <c r="A8" s="57"/>
-      <c r="B8" s="58" t="s">
+      <c r="A8" s="53"/>
+      <c r="B8" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="59">
+      <c r="C8" s="55">
         <v>2</v>
       </c>
-      <c r="D8" s="59">
+      <c r="D8" s="55">
         <v>124</v>
       </c>
-      <c r="E8" s="60">
+      <c r="E8" s="56">
         <v>248</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1" spans="2:5">
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="59">
+      <c r="C9" s="55">
         <v>2</v>
       </c>
-      <c r="D9" s="59">
+      <c r="D9" s="55">
         <v>134</v>
       </c>
-      <c r="E9" s="60">
+      <c r="E9" s="56">
         <v>268</v>
       </c>
     </row>
     <row r="10" ht="19" customHeight="1" spans="2:5">
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="62">
+      <c r="C10" s="58">
         <v>4</v>
       </c>
-      <c r="D10" s="62">
+      <c r="D10" s="58">
         <v>14</v>
       </c>
-      <c r="E10" s="63">
+      <c r="E10" s="59">
         <v>56</v>
       </c>
     </row>
     <row r="11" ht="19" customHeight="1" spans="2:5">
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="65">
+      <c r="C11" s="61">
         <v>24</v>
       </c>
-      <c r="D11" s="65">
+      <c r="D11" s="61">
         <v>4</v>
       </c>
-      <c r="E11" s="66">
+      <c r="E11" s="62">
         <v>96</v>
       </c>
     </row>
     <row r="12" ht="19" customHeight="1" spans="2:5">
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="68">
+      <c r="D12" s="64">
         <v>100</v>
       </c>
-      <c r="E12" s="69">
+      <c r="E12" s="65">
         <v>200</v>
       </c>
     </row>
     <row r="13" ht="19" customHeight="1" spans="2:5">
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="68">
+      <c r="C13" s="64">
         <v>8</v>
       </c>
-      <c r="D13" s="68">
+      <c r="D13" s="64">
         <v>9</v>
       </c>
-      <c r="E13" s="69">
+      <c r="E13" s="65">
         <v>72</v>
       </c>
     </row>
     <row r="14" ht="19" customHeight="1" spans="2:5">
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="68">
+      <c r="C14" s="64">
         <v>1</v>
       </c>
-      <c r="D14" s="68">
+      <c r="D14" s="64">
         <v>22</v>
       </c>
-      <c r="E14" s="69">
+      <c r="E14" s="65">
         <v>22</v>
       </c>
     </row>
     <row r="15" ht="13.5" spans="2:5">
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="72">
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="68">
         <f>SUM(E7:E14)</f>
         <v>1362</v>
       </c>
     </row>
     <row r="32" spans="2:3">
-      <c r="B32" s="73"/>
-      <c r="C32" s="73"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
     </row>
     <row r="33" spans="2:3">
-      <c r="B33" s="73"/>
-      <c r="C33" s="73"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
     </row>
     <row r="34" spans="2:3">
-      <c r="B34" s="73"/>
-      <c r="C34" s="73"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
     </row>
     <row r="35" spans="2:3">
-      <c r="B35" s="73"/>
-      <c r="C35" s="73"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
     </row>
     <row r="36" spans="2:3">
-      <c r="B36" s="73"/>
-      <c r="C36" s="73"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="69"/>
     </row>
     <row r="44" ht="19.5" spans="10:10">
       <c r="J44" s="12" t="s">
@@ -2123,8 +2123,8 @@
       <c r="B6">
         <v>10</v>
       </c>
-      <c r="O6" s="50"/>
-      <c r="P6" s="50"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
@@ -2218,178 +2218,178 @@
       <c r="H7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="43" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:9">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="20">
         <v>1</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <f>(D37)</f>
         <v>358</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="21">
         <f t="shared" ref="E8:E14" si="0">(C8*D8)</f>
         <v>358</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="48"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="44"/>
     </row>
     <row r="9" spans="2:9">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="20">
         <v>1</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="20">
         <v>134</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="21">
         <f t="shared" si="0"/>
         <v>134</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="48">
+      <c r="I9" s="44">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:9">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="20">
         <v>4</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <v>14</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="21">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="48">
+      <c r="I10" s="44">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:9">
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="20">
         <v>12</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="20">
         <v>4</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="21">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="44" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="20">
         <v>1</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="20">
         <v>100</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="21">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="48" t="s">
+      <c r="I12" s="44" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="20">
         <v>8</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="20">
         <v>9</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="21">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="48">
+      <c r="I13" s="44">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:9">
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="20">
         <v>1</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="20">
         <v>22</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="21">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="49" t="s">
+      <c r="H14" s="26"/>
+      <c r="I14" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30">
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29">
         <f>SUM(E8:E14)</f>
         <v>790</v>
       </c>
@@ -2401,27 +2401,27 @@
       <c r="B17" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="31" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" ht="17.25" spans="2:9">
-      <c r="B18" s="20" t="s">
+    <row r="18" spans="2:9">
+      <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="20">
         <v>1</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="20">
         <v>500</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="21">
         <f t="shared" ref="E18:E24" si="1">(C18*D18)</f>
         <v>500</v>
       </c>
@@ -2429,121 +2429,121 @@
       <c r="H18"/>
       <c r="I18"/>
     </row>
-    <row r="19" ht="17.25" spans="2:5">
-      <c r="B19" s="25" t="s">
+    <row r="19" spans="2:5">
+      <c r="B19" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="20">
         <v>1</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="20">
         <v>134</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="21">
         <f t="shared" si="1"/>
         <v>134</v>
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="20">
         <v>4</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="20">
         <v>14</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="21">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="20">
         <v>12</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="20">
         <v>4</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="21">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="20">
         <v>8</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="20">
         <v>9</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="21">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="20">
         <v>1</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="20">
         <v>22</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="21">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="20">
         <v>1</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="20">
         <v>100</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="21">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="33"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="35"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="33"/>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="33"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="35"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="33"/>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="38">
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="29">
         <f>SUM(E18:E24)</f>
         <v>932</v>
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C29" s="3"/>
@@ -2551,22 +2551,22 @@
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="41" t="s">
+      <c r="C30" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="41" t="s">
+      <c r="D30" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="42"/>
+      <c r="E30" s="38"/>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="42"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="38"/>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="5" t="s">
@@ -2623,15 +2623,15 @@
       <c r="E36" s="7"/>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="44"/>
-      <c r="D37" s="45">
+      <c r="C37" s="40"/>
+      <c r="D37" s="41">
         <f>SUM(D32:D35)</f>
         <v>358</v>
       </c>
-      <c r="E37" s="46"/>
+      <c r="E37" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2645,18 +2645,18 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="92.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="88.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="97.3583333333333" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" spans="1:3">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -2667,12 +2667,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" ht="16.5" spans="1:3">
+    <row r="2" spans="1:3">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
     </row>
-    <row r="3" ht="16.5" spans="1:3">
+    <row r="3" spans="1:3">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" ht="16.5" spans="1:3">
+    <row r="4" spans="1:3">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" ht="16.5" spans="1:3">
+    <row r="5" spans="1:3">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" ht="16.5" spans="1:3">
+    <row r="6" spans="1:3">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" ht="16.5" spans="1:3">
+    <row r="7" spans="1:3">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -2727,84 +2727,91 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" ht="16.5" spans="1:3">
+    <row r="8" spans="1:3">
       <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" ht="16.5" spans="1:3">
+      <c r="B8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" ht="16.5" spans="1:3">
+      <c r="B9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="6"/>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" ht="16.5" spans="1:3">
+    <row r="11" spans="1:3">
       <c r="A11" s="8">
         <v>9</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" ht="16.5" spans="1:3">
+    <row r="12" spans="1:3">
       <c r="A12" s="8">
         <v>10</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
     </row>
-    <row r="13" ht="16.5" spans="1:3">
+    <row r="13" spans="1:3">
       <c r="A13" s="8">
         <v>11</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
     </row>
-    <row r="14" ht="16.5" spans="1:3">
+    <row r="14" spans="1:3">
       <c r="A14" s="8">
         <v>12</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" ht="16.5" spans="1:3">
+    <row r="15" spans="1:3">
       <c r="A15" s="8">
         <v>13</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" ht="16.5" spans="1:3">
+    <row r="16" spans="1:3">
       <c r="A16" s="8">
         <v>14</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" ht="16.5" spans="1:3">
+    <row r="17" spans="1:3">
       <c r="A17" s="8">
         <v>15</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" ht="16.5" spans="1:3">
+    <row r="18" spans="1:3">
       <c r="A18" s="8">
         <v>16</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
     </row>
-    <row r="19" ht="16.5" spans="1:3">
+    <row r="19" spans="1:3">
       <c r="A19" s="9">
         <v>17</v>
       </c>

</xml_diff>